<commit_message>
Added excel reading and write
</commit_message>
<xml_diff>
--- a/DB/Excel1.xlsx
+++ b/DB/Excel1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\BitBucket\GITPOC\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228173D3-78CC-4BA0-A118-CCD4DC26EDD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943BA0DD-7F67-4AD7-9014-F1EEAB1B82BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2068FFFB-3467-4DB4-9382-AB1B5E8D46DF}"/>
+    <workbookView xWindow="8640" yWindow="2124" windowWidth="11712" windowHeight="8964" activeTab="1" xr2:uid="{2068FFFB-3467-4DB4-9382-AB1B5E8D46DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,12 +32,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>One</t>
   </si>
   <si>
     <t>two</t>
+  </si>
+  <si>
+    <t>https://www.nseindia.com/live_market/dynaContent/live_watch/get_quote/GetQuoteFO.jsp?underlying=SUNPHARMA&amp;instrument=OPTSTK&amp;strike=400.00&amp;type=PE&amp;expiry=25JUL2019</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>26.00</t>
+  </si>
+  <si>
+    <t>dsadsckank</t>
   </si>
 </sst>
 </file>
@@ -72,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B5DF1E-3EF5-4E90-A561-578326032A37}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -412,4 +432,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49227E8A-FC81-4B55-B69A-FAE3136FDE5B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>